<commit_message>
add: create resource controller
</commit_message>
<xml_diff>
--- a/comandos laravel.xlsx
+++ b/comandos laravel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodeghiero/developer/courses/laravel-course/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F47605D8-456B-B84F-81E9-50B8E6DAC44D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349065C8-3D69-6847-9A26-C466A439A516}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">List!$3:$3</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,26 +28,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>TASK OR TITLE</t>
   </si>
   <si>
-    <t>ITEM</t>
-  </si>
-  <si>
     <t>NOTES</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
     <t>Commands</t>
   </si>
   <si>
@@ -64,6 +52,21 @@
   </si>
   <si>
     <t>listar tabela de rotas</t>
+  </si>
+  <si>
+    <t>php artisan make:controller clienteControlador --resource</t>
+  </si>
+  <si>
+    <t>cria um controlador pré configurado</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">php artisan make:controller clienteControlador </t>
+  </si>
+  <si>
+    <t>cria um controlador simples</t>
   </si>
 </sst>
 </file>
@@ -236,7 +239,7 @@
   <autoFilter ref="B3:D7" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Commands" dataCellStyle="Date"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ITEM"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column1"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="NOTES"/>
   </tableColumns>
   <tableStyleInfo name="Tasks" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -518,15 +521,15 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="41" customWidth="1"/>
+    <col min="2" max="2" width="51.1640625" customWidth="1"/>
     <col min="3" max="3" width="32.5" customWidth="1"/>
-    <col min="4" max="4" width="29.5" customWidth="1"/>
+    <col min="4" max="4" width="37.83203125" customWidth="1"/>
     <col min="5" max="5" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -538,62 +541,54 @@
     </row>
     <row r="2" spans="1:4" ht="24" x14ac:dyDescent="0.15">
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="22.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>4</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>4</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>